<commit_message>
Teodepago BETA Funcional v1.
</commit_message>
<xml_diff>
--- a/src/Services/usuarios.xlsx
+++ b/src/Services/usuarios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20414"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\teodepagos\src\Services\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{635E402B-6C81-4948-BA57-F10F35CE7BCB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91DDD129-808E-491D-8881-EA31071C7C6B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{C3CB8991-09D1-4F35-B378-62C6011C30C3}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{C3CB8991-09D1-4F35-B378-62C6011C30C3}"/>
   </bookViews>
   <sheets>
     <sheet name="usuarios" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1152" uniqueCount="721">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1162" uniqueCount="722">
   <si>
     <t>nombre_apellido</t>
   </si>
@@ -2115,86 +2115,89 @@
     <t>19122009</t>
   </si>
   <si>
-    <t>48540634</t>
-  </si>
-  <si>
-    <t>49393473</t>
-  </si>
-  <si>
-    <t>49271791</t>
-  </si>
-  <si>
-    <t>49202241</t>
-  </si>
-  <si>
-    <t>49271653</t>
-  </si>
-  <si>
-    <t>48748072</t>
-  </si>
-  <si>
-    <t>48738437</t>
-  </si>
-  <si>
-    <t>48747890</t>
-  </si>
-  <si>
-    <t>47770732</t>
-  </si>
-  <si>
-    <t>49202659</t>
-  </si>
-  <si>
-    <t>70000401</t>
-  </si>
-  <si>
-    <t>70000402</t>
-  </si>
-  <si>
-    <t>70000403</t>
-  </si>
-  <si>
-    <t>70000404</t>
-  </si>
-  <si>
-    <t>70000405</t>
-  </si>
-  <si>
-    <t>70000406</t>
-  </si>
-  <si>
-    <t>70000407</t>
-  </si>
-  <si>
-    <t>50100000</t>
-  </si>
-  <si>
-    <t>50200000</t>
-  </si>
-  <si>
-    <t>50300000</t>
-  </si>
-  <si>
-    <t>50400000</t>
-  </si>
-  <si>
-    <t>50500000</t>
-  </si>
-  <si>
-    <t>50600000</t>
-  </si>
-  <si>
-    <t>50700000</t>
-  </si>
-  <si>
-    <t>50800000</t>
+    <t>06012009</t>
+  </si>
+  <si>
+    <t>09022009</t>
+  </si>
+  <si>
+    <t>27022009</t>
+  </si>
+  <si>
+    <t>07022009</t>
+  </si>
+  <si>
+    <t>12102008</t>
+  </si>
+  <si>
+    <t>12092008</t>
+  </si>
+  <si>
+    <t>26032007</t>
+  </si>
+  <si>
+    <t>19022009</t>
+  </si>
+  <si>
+    <t>17012008</t>
+  </si>
+  <si>
+    <t>09112007</t>
+  </si>
+  <si>
+    <t>30072007</t>
+  </si>
+  <si>
+    <t>25022008</t>
+  </si>
+  <si>
+    <t>14112006</t>
+  </si>
+  <si>
+    <t>24032007</t>
+  </si>
+  <si>
+    <t>30032007</t>
+  </si>
+  <si>
+    <t>07122006</t>
+  </si>
+  <si>
+    <t>28052007</t>
+  </si>
+  <si>
+    <t>08032007</t>
+  </si>
+  <si>
+    <t>26102006</t>
+  </si>
+  <si>
+    <t>Javier Caceres</t>
+  </si>
+  <si>
+    <t>Nahuel Andrade</t>
+  </si>
+  <si>
+    <t>Nahuel Crocombete</t>
+  </si>
+  <si>
+    <t>3595</t>
+  </si>
+  <si>
+    <t>12052002</t>
+  </si>
+  <si>
+    <t>12112002</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2208,6 +2211,23 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF212121"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -2233,10 +2253,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2259,9 +2280,19 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2574,10 +2605,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7557DFF3-677F-4336-ADBF-1E30464B0F93}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:J383"/>
+  <dimension ref="A1:J386"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A359" workbookViewId="0">
-      <selection activeCell="H371" sqref="H371"/>
+    <sheetView tabSelected="1" topLeftCell="A357" workbookViewId="0">
+      <selection activeCell="F385" sqref="F385"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9395,8 +9426,8 @@
       <c r="B359">
         <v>48540634</v>
       </c>
-      <c r="C359" s="9" t="s">
-        <v>696</v>
+      <c r="C359" s="10" t="s">
+        <v>683</v>
       </c>
       <c r="D359" t="s">
         <v>628</v>
@@ -9407,7 +9438,7 @@
       <c r="F359" s="4">
         <v>0</v>
       </c>
-      <c r="G359" s="4"/>
+      <c r="G359" s="10"/>
     </row>
     <row r="360" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A360" s="5" t="s">
@@ -9416,8 +9447,8 @@
       <c r="B360">
         <v>49393473</v>
       </c>
-      <c r="C360" s="9" t="s">
-        <v>697</v>
+      <c r="C360" s="10" t="s">
+        <v>696</v>
       </c>
       <c r="D360" s="4" t="s">
         <v>628</v>
@@ -9428,7 +9459,7 @@
       <c r="F360" s="4">
         <v>0</v>
       </c>
-      <c r="G360" s="4"/>
+      <c r="G360" s="10"/>
       <c r="H360" s="4"/>
       <c r="J360" s="4"/>
     </row>
@@ -9439,8 +9470,8 @@
       <c r="B361">
         <v>49271791</v>
       </c>
-      <c r="C361" s="9" t="s">
-        <v>698</v>
+      <c r="C361" s="10" t="s">
+        <v>697</v>
       </c>
       <c r="D361" s="4" t="s">
         <v>628</v>
@@ -9451,7 +9482,7 @@
       <c r="F361" s="4">
         <v>0</v>
       </c>
-      <c r="G361" s="4"/>
+      <c r="G361" s="10"/>
       <c r="H361" s="4"/>
       <c r="J361" s="4"/>
     </row>
@@ -9462,8 +9493,8 @@
       <c r="B362">
         <v>49202241</v>
       </c>
-      <c r="C362" s="9" t="s">
-        <v>699</v>
+      <c r="C362" s="10" t="s">
+        <v>698</v>
       </c>
       <c r="D362" s="4" t="s">
         <v>628</v>
@@ -9474,7 +9505,7 @@
       <c r="F362" s="4">
         <v>0</v>
       </c>
-      <c r="G362" s="4"/>
+      <c r="G362" s="10"/>
       <c r="H362" s="4"/>
       <c r="J362" s="4"/>
     </row>
@@ -9485,8 +9516,8 @@
       <c r="B363">
         <v>49271653</v>
       </c>
-      <c r="C363" s="9" t="s">
-        <v>700</v>
+      <c r="C363" s="10" t="s">
+        <v>699</v>
       </c>
       <c r="D363" s="4" t="s">
         <v>628</v>
@@ -9497,7 +9528,7 @@
       <c r="F363" s="4">
         <v>0</v>
       </c>
-      <c r="G363" s="4"/>
+      <c r="G363" s="10"/>
       <c r="H363" s="4"/>
       <c r="J363" s="4"/>
     </row>
@@ -9508,8 +9539,8 @@
       <c r="B364">
         <v>48748072</v>
       </c>
-      <c r="C364" s="9" t="s">
-        <v>701</v>
+      <c r="C364" s="10" t="s">
+        <v>700</v>
       </c>
       <c r="D364" s="4" t="s">
         <v>628</v>
@@ -9520,7 +9551,7 @@
       <c r="F364" s="4">
         <v>0</v>
       </c>
-      <c r="G364" s="4"/>
+      <c r="G364" s="10"/>
       <c r="H364" s="4"/>
       <c r="J364" s="4"/>
     </row>
@@ -9531,8 +9562,8 @@
       <c r="B365">
         <v>48738437</v>
       </c>
-      <c r="C365" s="9" t="s">
-        <v>702</v>
+      <c r="C365" s="10" t="s">
+        <v>222</v>
       </c>
       <c r="D365" s="4" t="s">
         <v>628</v>
@@ -9543,7 +9574,7 @@
       <c r="F365" s="4">
         <v>0</v>
       </c>
-      <c r="G365" s="4"/>
+      <c r="G365" s="10"/>
       <c r="H365" s="4"/>
       <c r="J365" s="4"/>
     </row>
@@ -9554,8 +9585,8 @@
       <c r="B366">
         <v>48747890</v>
       </c>
-      <c r="C366" s="9" t="s">
-        <v>703</v>
+      <c r="C366" s="10" t="s">
+        <v>701</v>
       </c>
       <c r="D366" s="4" t="s">
         <v>628</v>
@@ -9566,7 +9597,7 @@
       <c r="F366" s="4">
         <v>0</v>
       </c>
-      <c r="G366" s="4"/>
+      <c r="G366" s="10"/>
       <c r="H366" s="4"/>
       <c r="J366" s="4"/>
     </row>
@@ -9577,8 +9608,8 @@
       <c r="B367">
         <v>47770732</v>
       </c>
-      <c r="C367" s="9" t="s">
-        <v>704</v>
+      <c r="C367" s="11" t="s">
+        <v>702</v>
       </c>
       <c r="D367" s="4" t="s">
         <v>628</v>
@@ -9589,7 +9620,7 @@
       <c r="F367" s="4">
         <v>0</v>
       </c>
-      <c r="G367" s="4"/>
+      <c r="G367" s="11"/>
       <c r="H367" s="4"/>
       <c r="J367" s="4"/>
     </row>
@@ -9600,8 +9631,8 @@
       <c r="B368">
         <v>49202659</v>
       </c>
-      <c r="C368" s="9" t="s">
-        <v>705</v>
+      <c r="C368" s="10" t="s">
+        <v>703</v>
       </c>
       <c r="D368" s="4" t="s">
         <v>628</v>
@@ -9612,7 +9643,7 @@
       <c r="F368" s="4">
         <v>0</v>
       </c>
-      <c r="G368" s="4"/>
+      <c r="G368" s="10"/>
       <c r="H368" s="4"/>
       <c r="J368" s="4"/>
     </row>
@@ -9623,8 +9654,8 @@
       <c r="B369">
         <v>70000401</v>
       </c>
-      <c r="C369" s="9" t="s">
-        <v>706</v>
+      <c r="C369" s="10" t="s">
+        <v>141</v>
       </c>
       <c r="D369" s="4" t="s">
         <v>628</v>
@@ -9635,7 +9666,7 @@
       <c r="F369" s="4">
         <v>0</v>
       </c>
-      <c r="G369" s="4"/>
+      <c r="G369" s="10"/>
       <c r="H369" s="4"/>
       <c r="J369" s="4"/>
     </row>
@@ -9646,8 +9677,8 @@
       <c r="B370">
         <v>70000402</v>
       </c>
-      <c r="C370" s="9" t="s">
-        <v>707</v>
+      <c r="C370" s="10" t="s">
+        <v>704</v>
       </c>
       <c r="D370" s="4" t="s">
         <v>628</v>
@@ -9658,7 +9689,7 @@
       <c r="F370" s="4">
         <v>0</v>
       </c>
-      <c r="G370" s="4"/>
+      <c r="G370" s="10"/>
       <c r="H370" s="4"/>
       <c r="J370" s="4"/>
     </row>
@@ -9669,8 +9700,8 @@
       <c r="B371">
         <v>70000403</v>
       </c>
-      <c r="C371" s="9" t="s">
-        <v>708</v>
+      <c r="C371" s="10" t="s">
+        <v>226</v>
       </c>
       <c r="D371" s="4" t="s">
         <v>628</v>
@@ -9681,7 +9712,7 @@
       <c r="F371" s="4">
         <v>0</v>
       </c>
-      <c r="G371" s="4"/>
+      <c r="G371" s="10"/>
       <c r="H371" s="4"/>
       <c r="J371" s="4"/>
     </row>
@@ -9692,8 +9723,8 @@
       <c r="B372">
         <v>70000404</v>
       </c>
-      <c r="C372" s="9" t="s">
-        <v>709</v>
+      <c r="C372" s="10" t="s">
+        <v>705</v>
       </c>
       <c r="D372" s="4" t="s">
         <v>628</v>
@@ -9704,7 +9735,7 @@
       <c r="F372" s="4">
         <v>0</v>
       </c>
-      <c r="G372" s="4"/>
+      <c r="G372" s="10"/>
       <c r="H372" s="4"/>
       <c r="J372" s="4"/>
     </row>
@@ -9715,8 +9746,8 @@
       <c r="B373">
         <v>70000405</v>
       </c>
-      <c r="C373" s="9" t="s">
-        <v>710</v>
+      <c r="C373" s="10" t="s">
+        <v>706</v>
       </c>
       <c r="D373" s="4" t="s">
         <v>628</v>
@@ -9727,7 +9758,7 @@
       <c r="F373" s="4">
         <v>0</v>
       </c>
-      <c r="G373" s="4"/>
+      <c r="G373" s="10"/>
       <c r="H373" s="4"/>
       <c r="J373" s="4"/>
     </row>
@@ -9738,8 +9769,8 @@
       <c r="B374">
         <v>70000406</v>
       </c>
-      <c r="C374" s="9" t="s">
-        <v>711</v>
+      <c r="C374" s="10" t="s">
+        <v>707</v>
       </c>
       <c r="D374" s="4" t="s">
         <v>628</v>
@@ -9750,7 +9781,7 @@
       <c r="F374" s="4">
         <v>0</v>
       </c>
-      <c r="G374" s="4"/>
+      <c r="G374" s="10"/>
       <c r="H374" s="4"/>
       <c r="J374" s="4"/>
     </row>
@@ -9761,8 +9792,8 @@
       <c r="B375">
         <v>70000407</v>
       </c>
-      <c r="C375" s="9" t="s">
-        <v>712</v>
+      <c r="C375" s="10" t="s">
+        <v>207</v>
       </c>
       <c r="D375" s="4" t="s">
         <v>628</v>
@@ -9773,7 +9804,7 @@
       <c r="F375" s="4">
         <v>0</v>
       </c>
-      <c r="G375" s="4"/>
+      <c r="G375" s="10"/>
       <c r="H375" s="4"/>
       <c r="J375" s="4"/>
     </row>
@@ -9784,8 +9815,8 @@
       <c r="B376">
         <v>50100000</v>
       </c>
-      <c r="C376" s="9" t="s">
-        <v>713</v>
+      <c r="C376" s="10" t="s">
+        <v>708</v>
       </c>
       <c r="D376" s="4" t="s">
         <v>628</v>
@@ -9796,7 +9827,7 @@
       <c r="F376" s="4">
         <v>0</v>
       </c>
-      <c r="G376" s="4"/>
+      <c r="G376" s="10"/>
       <c r="H376" s="4"/>
       <c r="J376" s="4"/>
     </row>
@@ -9807,8 +9838,8 @@
       <c r="B377">
         <v>50200000</v>
       </c>
-      <c r="C377" s="9" t="s">
-        <v>714</v>
+      <c r="C377" s="10" t="s">
+        <v>709</v>
       </c>
       <c r="D377" s="4" t="s">
         <v>628</v>
@@ -9819,7 +9850,7 @@
       <c r="F377" s="4">
         <v>0</v>
       </c>
-      <c r="G377" s="4"/>
+      <c r="G377" s="10"/>
       <c r="H377" s="4"/>
       <c r="J377" s="4"/>
     </row>
@@ -9830,8 +9861,8 @@
       <c r="B378">
         <v>50300000</v>
       </c>
-      <c r="C378" s="9" t="s">
-        <v>715</v>
+      <c r="C378" s="10" t="s">
+        <v>710</v>
       </c>
       <c r="D378" s="4" t="s">
         <v>628</v>
@@ -9842,7 +9873,7 @@
       <c r="F378" s="4">
         <v>0</v>
       </c>
-      <c r="G378" s="4"/>
+      <c r="G378" s="10"/>
       <c r="H378" s="4"/>
       <c r="J378" s="4"/>
     </row>
@@ -9853,8 +9884,8 @@
       <c r="B379">
         <v>50400000</v>
       </c>
-      <c r="C379" s="9" t="s">
-        <v>716</v>
+      <c r="C379" s="10" t="s">
+        <v>709</v>
       </c>
       <c r="D379" s="4" t="s">
         <v>628</v>
@@ -9865,7 +9896,7 @@
       <c r="F379" s="4">
         <v>0</v>
       </c>
-      <c r="G379" s="4"/>
+      <c r="G379" s="10"/>
       <c r="H379" s="4"/>
       <c r="J379" s="4"/>
     </row>
@@ -9876,8 +9907,8 @@
       <c r="B380">
         <v>50500000</v>
       </c>
-      <c r="C380" s="9" t="s">
-        <v>717</v>
+      <c r="C380" s="10" t="s">
+        <v>711</v>
       </c>
       <c r="D380" s="4" t="s">
         <v>628</v>
@@ -9888,7 +9919,7 @@
       <c r="F380" s="4">
         <v>0</v>
       </c>
-      <c r="G380" s="4"/>
+      <c r="G380" s="10"/>
       <c r="H380" s="4"/>
       <c r="J380" s="4"/>
     </row>
@@ -9899,8 +9930,8 @@
       <c r="B381">
         <v>50600000</v>
       </c>
-      <c r="C381" s="9" t="s">
-        <v>718</v>
+      <c r="C381" s="10" t="s">
+        <v>712</v>
       </c>
       <c r="D381" s="4" t="s">
         <v>628</v>
@@ -9911,7 +9942,7 @@
       <c r="F381" s="4">
         <v>0</v>
       </c>
-      <c r="G381" s="4"/>
+      <c r="G381" s="10"/>
       <c r="H381" s="4"/>
       <c r="J381" s="4"/>
     </row>
@@ -9922,8 +9953,8 @@
       <c r="B382">
         <v>50700000</v>
       </c>
-      <c r="C382" s="9" t="s">
-        <v>719</v>
+      <c r="C382" s="10" t="s">
+        <v>713</v>
       </c>
       <c r="D382" s="4" t="s">
         <v>628</v>
@@ -9934,7 +9965,7 @@
       <c r="F382" s="4">
         <v>0</v>
       </c>
-      <c r="G382" s="4"/>
+      <c r="G382" s="10"/>
       <c r="H382" s="4"/>
       <c r="J382" s="4"/>
     </row>
@@ -9945,8 +9976,8 @@
       <c r="B383">
         <v>50800000</v>
       </c>
-      <c r="C383" s="9" t="s">
-        <v>720</v>
+      <c r="C383" s="10" t="s">
+        <v>714</v>
       </c>
       <c r="D383" s="4" t="s">
         <v>628</v>
@@ -9957,9 +9988,63 @@
       <c r="F383" s="4">
         <v>0</v>
       </c>
-      <c r="G383" s="4"/>
+      <c r="G383" s="10"/>
       <c r="H383" s="4"/>
       <c r="J383" s="4"/>
+    </row>
+    <row r="384" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A384" s="12" t="s">
+        <v>715</v>
+      </c>
+      <c r="B384">
+        <v>42926423</v>
+      </c>
+      <c r="C384" s="9" t="s">
+        <v>718</v>
+      </c>
+      <c r="D384" t="s">
+        <v>245</v>
+      </c>
+      <c r="F384">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="385" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A385" s="12" t="s">
+        <v>716</v>
+      </c>
+      <c r="B385">
+        <v>44429156</v>
+      </c>
+      <c r="C385" s="9" t="s">
+        <v>720</v>
+      </c>
+      <c r="D385" t="s">
+        <v>245</v>
+      </c>
+      <c r="E385" t="s">
+        <v>721</v>
+      </c>
+      <c r="F385">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="386" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A386" s="12" t="s">
+        <v>717</v>
+      </c>
+      <c r="B386">
+        <v>43992532</v>
+      </c>
+      <c r="C386" s="9" t="s">
+        <v>719</v>
+      </c>
+      <c r="D386" t="s">
+        <v>245</v>
+      </c>
+      <c r="F386">
+        <v>20000</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>